<commit_message>
- Plant excel changes
</commit_message>
<xml_diff>
--- a/assets/excels/PlantExcelSheet.xlsx
+++ b/assets/excels/PlantExcelSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\greenworld\assets\excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ajaj Patel.DESKTOP-N40AHF1\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,15 +24,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>QRCode</t>
-  </si>
-  <si>
-    <t>Description</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Plant(local name)</t>
+  </si>
+  <si>
+    <t>English name</t>
+  </si>
+  <si>
+    <t>Botanical name</t>
+  </si>
+  <si>
+    <t>Habit</t>
+  </si>
+  <si>
+    <t>Family</t>
+  </si>
+  <si>
+    <t>Watering</t>
+  </si>
+  <si>
+    <t>Location(indoor/outdoor)</t>
+  </si>
+  <si>
+    <t>Use</t>
+  </si>
+  <si>
+    <t>Extra Comment</t>
+  </si>
+  <si>
+    <t>Category</t>
   </si>
 </sst>
 </file>
@@ -359,18 +380,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -379,6 +409,27 @@
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>